<commit_message>
Fix relatedTo to relatedto c0267326c42093614dbaf24c5f351dd516a469de
</commit_message>
<xml_diff>
--- a/PriseEnCompteIssuesSurPublication20240918/ig/PN13-FHIR-prescmed-medicationrequest-conceptmap.xlsx
+++ b/PriseEnCompteIssuesSurPublication20240918/ig/PN13-FHIR-prescmed-medicationrequest-conceptmap.xlsx
@@ -9,12 +9,15 @@
     <sheet name="Metadata" r:id="rId3" sheetId="1"/>
     <sheet name="Mapping Table 0" r:id="rId4" sheetId="2"/>
     <sheet name="Mapping Table 1" r:id="rId5" sheetId="3"/>
+    <sheet name="Mapping Table 2" r:id="rId6" sheetId="4"/>
+    <sheet name="Mapping Table 3" r:id="rId7" sheetId="5"/>
+    <sheet name="Mapping Table 4" r:id="rId8" sheetId="6"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="67">
   <si>
     <t>Property</t>
   </si>
@@ -58,7 +61,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-09-18T15:06:02+00:00</t>
+    <t>2024-10-21T12:37:12+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -124,13 +127,97 @@
     <t>MedicationRequest.identifier.system</t>
   </si>
   <si>
-    <t>Messages/M_prescription_médicaments/Prescription/Elément_prescr_médic/Type_élément_prescr</t>
+    <t>Messages/M_prescription_médicaments/Prescription/Elément_prescr_médic/Libellé_élément_prescr</t>
+  </si>
+  <si>
+    <t>MedicationRequest.text</t>
+  </si>
+  <si>
+    <t>Messages/M_prescription_médicaments/Prescription/Elément_prescr_médic/Urgent</t>
+  </si>
+  <si>
+    <t>MedicationRequest.priority</t>
+  </si>
+  <si>
+    <t>Messages/M_prescription_médicaments/Prescription/Elément_prescr_médic/Voie_administration</t>
+  </si>
+  <si>
+    <t>MedicationRequest.dosageInstruction.route.coding.code</t>
+  </si>
+  <si>
+    <t>Messages/M_prescription_médicaments/Prescription/Elément_prescr_médic/Lieu_administration</t>
+  </si>
+  <si>
+    <t>MedicationRequest.dispenseRequest.performer.display</t>
+  </si>
+  <si>
+    <t>Messages/M_prescription_médicaments/Prescription/Elément_prescr_médic/Dispositif_associé</t>
+  </si>
+  <si>
+    <t>MedicationRequest.supportingInformation.display</t>
+  </si>
+  <si>
+    <t>Messages/M_prescription_médicaments/Prescription/Elément_prescr_médic/Commentaire</t>
+  </si>
+  <si>
+    <t>MedicationRequest.note.text</t>
+  </si>
+  <si>
+    <t>Messages/M_prescription_médicaments/Prescription/Elément_prescr_médic/Commentaire_structuré/Identification_auteur/Identifiant</t>
+  </si>
+  <si>
+    <t>MedicationRequest.note.authorReference.identifier.value</t>
+  </si>
+  <si>
+    <t>Messages/M_prescription_médicaments/Prescription/Elément_prescr_médic/Commentaire_structuré/Identification_auteur/Domaine_identification</t>
+  </si>
+  <si>
+    <t>MedicationRequest.note.authorReference.identifier.system</t>
+  </si>
+  <si>
+    <t>Messages/M_prescription_médicaments/Prescription/Elément_prescr_médic/Commentaire_structuré/Identification_auteur/Nom_usage</t>
   </si>
   <si>
     <t>related-to</t>
   </si>
   <si>
-    <t>MedicationRequest.medicationReference.reference</t>
+    <t>MedicationRequest.note.authorReference.display</t>
+  </si>
+  <si>
+    <t>Messages/M_prescription_médicaments/Prescription/Elément_prescr_médic/Commentaire_structuré/Identification_auteur/Prénom_usage</t>
+  </si>
+  <si>
+    <t>Messages/M_prescription_médicaments/Prescription/Elément_prescr_médic/Commentaire_structuré/Identification_auteur/Initiales</t>
+  </si>
+  <si>
+    <t>Messages/M_prescription_médicaments/Prescription/Elément_prescr_médic/Commentaire_structuré/Identification_auteur/Civilité</t>
+  </si>
+  <si>
+    <t>Messages/M_prescription_médicaments/Prescription/Elément_prescr_médic/Commentaire_structuré/Identification_auteur/Titre</t>
+  </si>
+  <si>
+    <t>Messages/M_prescription_médicaments/Prescription/Elément_prescr_médic/Commentaire_structuré/Identification_auteur/Nom_famille</t>
+  </si>
+  <si>
+    <t>Messages/M_prescription_médicaments/Prescription/Elément_prescr_médic/Commentaire_structuré/Identification_auteur/Prénoms</t>
+  </si>
+  <si>
+    <t>Messages/M_prescription_médicaments/Prescription/Elément_prescr_médic/Commentaire_structuré/Texte</t>
+  </si>
+  <si>
+    <t>Messages/M_prescription_médicaments/Prescription/Elément_prescr_médic/GoNogo</t>
+  </si>
+  <si>
+    <t>MedicationRequest.status</t>
+  </si>
+  <si>
+    <t>Messages/M_prescription_médicaments/Prescription/Elément_prescr_médic/Motif_attente</t>
+  </si>
+  <si>
+    <t>MedicationRequest.statusReason.text</t>
+  </si>
+  <si>
+    <t>Messages/M_prescription_médicaments/Prescription/Elément_prescr_médic/Conditions_application</t>
   </si>
 </sst>
 </file>
@@ -472,6 +559,140 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="1">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s" s="1">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s" s="1">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2"/>
+      <c r="B2" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" t="s" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="D4" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="D6" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="D9" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="E9" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -510,16 +731,323 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" t="s" s="2">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="E3" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="1">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s" s="1">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s" s="1">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2"/>
+      <c r="B2" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" t="s" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="D4" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="D5" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="D6" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="D7" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="2">
+        <v>57</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="D8" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="2">
+        <v>58</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="D9" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="2">
+        <v>59</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="D10" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="2">
+        <v>60</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="D11" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="2">
+        <v>61</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="D12" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="E12" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="1">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s" s="1">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s" s="1">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2"/>
+      <c r="B2" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" t="s" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="2">
+        <v>62</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="2">
+        <v>62</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="D4" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="2">
+        <v>62</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="2">
+        <v>62</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="D6" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="2">
+        <v>62</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="2">
+        <v>64</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="2">
+        <v>66</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="D9" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="E9" s="2"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>